<commit_message>
correciones del reporte mensual
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meliton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{419CBBD3-E59B-4737-BF40-4258036F99BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60043F07-7FAA-4A0A-80A2-8D57E1D55FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -95,16 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Señora</t>
-  </si>
-  <si>
-    <t>Virginia Angélica Barreda Grados</t>
-  </si>
-  <si>
-    <t>Gerente de División de Supervisión de Gas Natural</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>OSINERGMIN</t>
   </si>
@@ -157,6 +148,9 @@
   </si>
   <si>
     <t>{{Periodo}}</t>
+  </si>
+  <si>
+    <t>{{Destinatario}}</t>
   </si>
 </sst>
 </file>
@@ -235,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -244,12 +238,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -844,7 +841,7 @@
   <dimension ref="A10:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A12" sqref="A12:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,48 +858,44 @@
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -914,7 +907,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -924,7 +917,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -934,7 +927,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -951,11 +944,11 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>11</v>
+      <c r="A21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -965,7 +958,7 @@
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
@@ -982,68 +975,69 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="str">
+      <c r="A27" s="9" t="str">
         <f>"Nos dirigimos a usted para adjuntarle la información mensual de consumo de Etilmercaptano efectuada por nuestra empresa UNNA ENERGIA S.A durante el mes de " &amp; $B$22 &amp; " , de acuerdo a lo establecido por Osinergmin."</f>
         <v>Nos dirigimos a usted para adjuntarle la información mensual de consumo de Etilmercaptano efectuada por nuestra empresa UNNA ENERGIA S.A durante el mes de {{Periodo}} , de acuerdo a lo establecido por Osinergmin.</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A27:F31"/>
+    <mergeCell ref="A12:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajuste reporte segunda hoja
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFF04D6-4506-4BCD-97D1-A5A5576B1D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB6DF27-C3A0-4148-89BE-79A830ECF66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>De nuestra consideración:</t>
   </si>
@@ -108,9 +108,6 @@
     <t>INFORME MENSUAL PARA EL MINISTERIO DE ENERGÍA Y MINAS</t>
   </si>
   <si>
-    <t>NOVIEMBRE DEL 2023</t>
-  </si>
-  <si>
     <t>DIRECCIÓN GENERAL DE HIDROCARBUROS (DGH)</t>
   </si>
   <si>
@@ -219,59 +216,62 @@
     <t xml:space="preserve"> BPD</t>
   </si>
   <si>
-    <t>{{RecepcionGasNaturalAsociado.LoteZ2B}}</t>
-  </si>
-  <si>
-    <t>{{RecepcionGasNaturalAsociado.LoteX}}</t>
-  </si>
-  <si>
-    <t>{{RecepcionGasNaturalAsociado.LoteVI}}</t>
-  </si>
-  <si>
-    <t>{{RecepcionGasNaturalAsociado.LoteI}}</t>
-  </si>
-  <si>
-    <t>{{RecepcionGasNaturalAsociado.LoteV}}</t>
-  </si>
-  <si>
-    <t>{{RecepcionGasNaturalAsociado.Total}}</t>
-  </si>
-  <si>
-    <t>{{UsoGas.Total}}</t>
-  </si>
-  <si>
-    <t>{{UsoGas.GasNaturalRestituido}}</t>
-  </si>
-  <si>
-    <t>{{UsoGas.ConsumoPropio}}</t>
-  </si>
-  <si>
-    <t>{{UsoGas.ConvertidoEnLgn}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.Glp}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.PromedioLiquidos}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.PropanoSaturado}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.ButanoSaturado}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.Hexano}}</t>
-  </si>
-  <si>
-    <t>{{ProduccionLiquidosGasNatural.Condensados}}</t>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.LoteX}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.LoteVI}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.LoteI}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.Total}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.UsoGas.GasNaturalRestituido}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.UsoGas.ConsumoPropio}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.UsoGas.ConvertidoEnLgn}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.UsoGas.Total}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.Glp}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.PropanoSaturado}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.ButanoSaturado}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.Hexano}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.Condensados}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.ProduccionLiquidosGasNatural.PromedioLiquidos}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.Periodo}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.LoteZ69}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin1.RecepcionGasNaturalAsociado.LoteIV}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,16 +310,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF3F4254"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -395,11 +387,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -420,16 +449,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -451,22 +479,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -603,8 +643,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -946,9 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02853BE-23F3-4FDB-A85E-D2B25CE2876F}">
   <dimension ref="B8:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -961,84 +999,84 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1056,11 +1094,11 @@
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1077,69 +1115,69 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="17"/>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="6"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -1150,14 +1188,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="17" t="s">
+      <c r="I30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="17"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
@@ -1170,41 +1208,41 @@
       <c r="B33" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -1228,68 +1266,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8B61D0-1E0A-46E2-B36D-518440A4EA7A}">
-  <dimension ref="B6:M45"/>
+  <dimension ref="B6:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="24" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J8" s="26" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="M8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="26"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1297,466 +1389,569 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="19" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="M19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="M20" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="16"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="27"/>
+      <c r="H21" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="21" t="s">
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="M29" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="27"/>
+      <c r="H33" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="23" t="s">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="27"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23" t="s">
+      <c r="G40" s="27"/>
+      <c r="H40" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+    </row>
+    <row r="41" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23" t="s">
+      <c r="G41" s="27"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="M34" s="13"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="23" t="s">
+      <c r="G42" s="27"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="21" t="s">
+      <c r="G43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="27"/>
+      <c r="H44" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="27"/>
+      <c r="H45" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="23"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="23"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G43" s="23"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" s="23"/>
-      <c r="H44" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="23"/>
-      <c r="H45" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H25:K25"/>
+  <mergeCells count="77">
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="H40:K40"/>
     <mergeCell ref="H41:K41"/>
@@ -1773,25 +1968,48 @@
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="M8:N10"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M29:N30"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Ajuste de datos cartas
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CBA16F-9583-4F10-9A32-8AA5B9712A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CEC39A-29C8-4603-A3B1-9D3C88B38DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>De nuestra consideración:</t>
   </si>
@@ -262,6 +263,88 @@
   </si>
   <si>
     <t>{{SitioWeb}}</t>
+  </si>
+  <si>
+    <t>UNNA ENERGIA</t>
+  </si>
+  <si>
+    <t>PLANTA DE DESTILACION VERDUN ALTO : 2,000 BARRILES</t>
+  </si>
+  <si>
+    <t>PLANTA DE ABSORCION PARIÑAS : 40 MMPCD</t>
+  </si>
+  <si>
+    <t>REPORTE MENSUAL</t>
+  </si>
+  <si>
+    <t>Articulo 7ºdel Reglamento de la Ley del Organismo Supervisor de la Inversión en Energía y Mineria D.S. 005-97-EM</t>
+  </si>
+  <si>
+    <t>RECUPERACION MENSUAL DE LIQUIDOS DEL GAS NATURAL ( BARRILES)</t>
+  </si>
+  <si>
+    <t>MES / PRODUCTO</t>
+  </si>
+  <si>
+    <t>PROPANO</t>
+  </si>
+  <si>
+    <t>BUTANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CGN(*)</t>
+  </si>
+  <si>
+    <t>SOLVENTE</t>
+  </si>
+  <si>
+    <t>TOTAL
+LGN</t>
+  </si>
+  <si>
+    <t>ENERO</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>MAYO</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>JULIO</t>
+  </si>
+  <si>
+    <t>AGOSTO</t>
+  </si>
+  <si>
+    <t>SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>DICIEMBRE</t>
+  </si>
+  <si>
+    <t>VENTA MENSUAL DE PRODUCTOS LIQUIDOS RECUPERADOS DEL GAS NATURAL (BARRILES)</t>
+  </si>
+  <si>
+    <t>EXISTENCIA MEDIA MENSUAL DE PRODUCTOS LIQUIDOS RECUPERADOS DEL GAS NATURAL (BARRILES)</t>
+  </si>
+  <si>
+    <t>NOTA: (*) CGN = Condensados del Gas Natural</t>
   </si>
 </sst>
 </file>
@@ -429,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -480,6 +563,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -492,54 +617,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,6 +794,55 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="309561" y="250032"/>
+          <a:ext cx="1472559" cy="547688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>448255</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C7D3CA-66E6-4EFE-8F0D-05C8E54D2BC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="200025"/>
           <a:ext cx="1472559" cy="547688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1007,9 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02853BE-23F3-4FDB-A85E-D2B25CE2876F}">
   <dimension ref="B8:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:J21"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1291,31 +1436,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8B61D0-1E0A-46E2-B36D-518440A4EA7A}">
   <dimension ref="B6:J49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:J20"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
@@ -1330,52 +1475,52 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
       <c r="I8" s="17" t="s">
         <v>65</v>
       </c>
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="12"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="14"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1393,28 +1538,34 @@
         <v>16</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="D13" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="D14" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="D15" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
@@ -1425,14 +1576,14 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
@@ -1445,110 +1596,110 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40" t="s">
+      <c r="E19" s="31"/>
+      <c r="F19" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="40"/>
+      <c r="G19" s="31"/>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="28" t="s">
+      <c r="E20" s="25"/>
+      <c r="F20" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="22"/>
       <c r="I20" s="18" t="s">
         <v>66</v>
       </c>
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="29" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="28" t="s">
+      <c r="E21" s="25"/>
+      <c r="F21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="22"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="23"/>
+      <c r="D22" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="28" t="s">
+      <c r="E22" s="25"/>
+      <c r="F22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="29" t="s">
+      <c r="C23" s="23"/>
+      <c r="D23" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="28" t="s">
+      <c r="E23" s="25"/>
+      <c r="F23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="29" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="28" t="s">
+      <c r="E24" s="25"/>
+      <c r="F24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26" t="s">
+      <c r="C25" s="39"/>
+      <c r="D25" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -1559,14 +1710,14 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
@@ -1579,96 +1730,96 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27" t="s">
+      <c r="E29" s="26"/>
+      <c r="F29" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="26"/>
       <c r="I29" s="18" t="s">
         <v>67</v>
       </c>
       <c r="J29" s="18"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="29" t="s">
+      <c r="C31" s="23"/>
+      <c r="D31" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="28" t="s">
+      <c r="E31" s="25"/>
+      <c r="F31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="28"/>
+      <c r="G31" s="22"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="29" t="s">
+      <c r="C32" s="23"/>
+      <c r="D32" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="28" t="s">
+      <c r="E32" s="25"/>
+      <c r="F32" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="29" t="s">
+      <c r="C33" s="23"/>
+      <c r="D33" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="28" t="s">
+      <c r="E33" s="25"/>
+      <c r="F33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="28"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="26" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -1679,14 +1830,14 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
@@ -1697,141 +1848,165 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27" t="s">
+      <c r="C39" s="26"/>
+      <c r="D39" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27" t="s">
+      <c r="E39" s="26"/>
+      <c r="F39" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="29" t="s">
+      <c r="C40" s="23"/>
+      <c r="D40" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="28" t="s">
+      <c r="E40" s="25"/>
+      <c r="F40" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="28"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="29" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="29" t="s">
+      <c r="C42" s="23"/>
+      <c r="D42" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="29" t="s">
+      <c r="C43" s="23"/>
+      <c r="D43" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="29" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="28" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="28"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="29" t="s">
+      <c r="C45" s="23"/>
+      <c r="D45" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="28" t="s">
+      <c r="E45" s="25"/>
+      <c r="F45" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="28"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="22"/>
+      <c r="C47" s="36"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
+  <mergeCells count="76">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:G49"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I29:J30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="F41:G41"/>
@@ -1848,51 +2023,674 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I29:J30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:G49"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5DB1-9EBB-48B8-AAC3-58813119E4A1}">
+  <dimension ref="B5:L52"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="K7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="12"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="8"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="B10" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48">
+        <v>0</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="50">
+        <v>21638.1</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="50">
+        <v>6936.58</v>
+      </c>
+      <c r="H21" s="48"/>
+      <c r="I21" s="50">
+        <v>28574.68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+    </row>
+    <row r="27" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="K27" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+    </row>
+    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+    </row>
+    <row r="32" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+    </row>
+    <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+    </row>
+    <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+    </row>
+    <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="50">
+        <v>21557.57</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="50">
+        <v>4904.3100000000004</v>
+      </c>
+      <c r="H35" s="48"/>
+    </row>
+    <row r="36" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+    </row>
+    <row r="40" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+    </row>
+    <row r="41" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+    </row>
+    <row r="42" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+    </row>
+    <row r="43" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+    </row>
+    <row r="44" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+    </row>
+    <row r="45" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+    </row>
+    <row r="46" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+    </row>
+    <row r="47" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+    </row>
+    <row r="48" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+    </row>
+    <row r="49" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="50">
+        <v>2598.4499999999998</v>
+      </c>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="50">
+        <v>2341.12</v>
+      </c>
+      <c r="H49" s="48"/>
+    </row>
+    <row r="50" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K7:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajuste cartas tercera hoja
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CEC39A-29C8-4603-A3B1-9D3C88B38DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7149F667-5DC5-4F61-9A10-AD8AC2DAE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Osinergmin2_Cgn">Hoja4!$B$36:$F$37</definedName>
+    <definedName name="Osinergmin2_Glp">Hoja4!$B$33:$F$34</definedName>
+    <definedName name="Osinergmin2_InventarioLiquidoGasNatural">Hoja4!$B$43:$F$44</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
   <si>
     <t>De nuestra consideración:</t>
   </si>
@@ -345,6 +351,63 @@
   </si>
   <si>
     <t>NOTA: (*) CGN = Condensados del Gas Natural</t>
+  </si>
+  <si>
+    <t>4,-VENTAS DE LIQUIDOS DEL GAS NATURAL</t>
+  </si>
+  <si>
+    <t>PRODUCTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PROPIEDADES Y CALIDAD</t>
+  </si>
+  <si>
+    <t>5,-VOLUMENES Y PERSONAS A LAS QUE SE VENDIERON LOS PRODUCTOS</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>6,-INVENTARIOS DE FIN DE MES DE LIQUIDOS DEL GAS NATURAL</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>{{item.Producto}}</t>
+  </si>
+  <si>
+    <t>{{item.Bls}}</t>
+  </si>
+  <si>
+    <t>CONDENSADOS DE GASOLINA</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.Glp}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.PropanoSaturado}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.ButanoSaturado}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.Hexano}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.CondensadoGasNatural}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.CondensadoGasolina}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.VentaLiquidoGasNatural.Total}}</t>
+  </si>
+  <si>
+    <t>GLP:</t>
+  </si>
+  <si>
+    <t>CGN:</t>
   </si>
 </sst>
 </file>
@@ -443,7 +506,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -508,11 +571,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -542,6 +618,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -563,81 +655,90 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,6 +908,55 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>709093</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C7A56F-BB2F-4A82-8FC1-71A3A719F84F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="352425"/>
+          <a:ext cx="1471093" cy="547688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1167,84 +1317,84 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1262,11 +1412,11 @@
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1283,69 +1433,69 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="20"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="18"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="6"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -1356,14 +1506,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="18"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
@@ -1376,41 +1526,41 @@
       <c r="B33" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -1436,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8B61D0-1E0A-46E2-B36D-518440A4EA7A}">
   <dimension ref="B6:J49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,14 +1603,14 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
@@ -1475,52 +1625,52 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="I8" s="17" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="I8" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="14"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1538,34 +1688,34 @@
         <v>16</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
@@ -1576,14 +1726,14 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
@@ -1596,110 +1746,110 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31" t="s">
+      <c r="C19" s="46"/>
+      <c r="D19" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31" t="s">
+      <c r="E19" s="46"/>
+      <c r="F19" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="46"/>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="45"/>
+      <c r="D20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="22" t="s">
+      <c r="E20" s="37"/>
+      <c r="F20" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="I20" s="18" t="s">
+      <c r="G20" s="36"/>
+      <c r="I20" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="J20" s="18"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="41"/>
+      <c r="D21" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="22" t="s">
+      <c r="E21" s="37"/>
+      <c r="F21" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="22"/>
+      <c r="G21" s="36"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="41"/>
+      <c r="D22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="37"/>
+      <c r="F22" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="22"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="25" t="s">
+      <c r="C23" s="41"/>
+      <c r="D23" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="22" t="s">
+      <c r="E23" s="37"/>
+      <c r="F23" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="22"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="25" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="37"/>
+      <c r="F24" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="22"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="33"/>
+      <c r="D25" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -1710,14 +1860,14 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
@@ -1730,96 +1880,96 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26" t="s">
+      <c r="E29" s="35"/>
+      <c r="F29" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="26"/>
-      <c r="I29" s="18" t="s">
+      <c r="G29" s="35"/>
+      <c r="I29" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="J29" s="18"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="25" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="37"/>
+      <c r="F31" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="22"/>
+      <c r="G31" s="36"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="25" t="s">
+      <c r="C32" s="41"/>
+      <c r="D32" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="37"/>
+      <c r="F32" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="22"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="25" t="s">
+      <c r="C33" s="41"/>
+      <c r="D33" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="22" t="s">
+      <c r="E33" s="37"/>
+      <c r="F33" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="22"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="27" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -1830,14 +1980,14 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
@@ -1848,123 +1998,183 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26" t="s">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26" t="s">
+      <c r="E39" s="35"/>
+      <c r="F39" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="26"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="25" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="22" t="s">
+      <c r="E40" s="37"/>
+      <c r="F40" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="22"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="25" t="s">
+      <c r="C41" s="41"/>
+      <c r="D41" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="25" t="s">
+      <c r="C42" s="41"/>
+      <c r="D42" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="25" t="s">
+      <c r="C43" s="41"/>
+      <c r="D43" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="25" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="22" t="s">
+      <c r="E44" s="37"/>
+      <c r="F44" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="22"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="25" t="s">
+      <c r="C45" s="41"/>
+      <c r="D45" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="22" t="s">
+      <c r="E45" s="37"/>
+      <c r="F45" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="22"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="36"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I29:J30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:G49"/>
     <mergeCell ref="B17:G17"/>
@@ -1981,66 +2191,6 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I29:J30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2049,10 +2199,520 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064DA171-C1CC-439E-88B1-52F94C095D82}">
+  <dimension ref="B5:L45"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="K7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="12"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="26"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="38"/>
+      <c r="G21" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="38"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="38"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="38"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="49"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="K27" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="26"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="33"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" s="33"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="38"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="38"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="57">
+        <f>SUM(SUM(E33:F34),SUM(E36:F37))</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="57"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="33"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I42" s="33"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="57">
+        <f>SUM(E43:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="58">
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="K7:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="H32:I37"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5DB1-9EBB-48B8-AAC3-58813119E4A1}">
   <dimension ref="B5:L52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2063,26 +2723,26 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -2090,169 +2750,169 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="K7" s="17" t="s">
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="K7" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="17"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="8"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="19" t="s">
         <v>79</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20">
         <v>0</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20">
         <v>0</v>
       </c>
       <c r="K17" s="4" t="s">
@@ -2261,425 +2921,425 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20">
         <v>0</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="18"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20">
         <v>0</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="21">
         <v>21638.1</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="50">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21">
         <v>6936.58</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="50">
+      <c r="H21" s="20"/>
+      <c r="I21" s="21">
         <v>28574.68</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48">
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="46" t="s">
+      <c r="H24" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="K27" s="18" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="K27" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="18"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
     </row>
     <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="21">
         <v>21557.57</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="50">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21">
         <v>4904.3100000000004</v>
       </c>
-      <c r="H35" s="48"/>
+      <c r="H35" s="20"/>
     </row>
     <row r="36" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="46" t="s">
+      <c r="F38" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="46" t="s">
+      <c r="G38" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="48" t="s">
+      <c r="B42" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
     </row>
     <row r="43" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
     </row>
     <row r="44" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
     </row>
     <row r="45" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
     </row>
     <row r="46" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
     </row>
     <row r="47" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
     </row>
     <row r="48" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
     </row>
     <row r="49" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="50">
+      <c r="C49" s="21">
         <v>2598.4499999999998</v>
       </c>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="50">
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="21">
         <v>2341.12</v>
       </c>
-      <c r="H49" s="48"/>
+      <c r="H49" s="20"/>
     </row>
     <row r="50" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="14" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajuste excel reporte cartas
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7149F667-5DC5-4F61-9A10-AD8AC2DAE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470425EF-1C7E-4A9F-946D-C0E8C87D88EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -588,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -655,6 +655,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -667,51 +709,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -727,18 +733,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02853BE-23F3-4FDB-A85E-D2B25CE2876F}">
   <dimension ref="B8:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1603,14 +1605,14 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
@@ -1625,39 +1627,39 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
       <c r="I8" s="25" t="s">
         <v>65</v>
       </c>
       <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="12"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
@@ -1726,14 +1728,14 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
@@ -1746,110 +1748,110 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46" t="s">
+      <c r="C19" s="39"/>
+      <c r="D19" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46" t="s">
+      <c r="E19" s="39"/>
+      <c r="F19" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="46"/>
+      <c r="G19" s="39"/>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="37" t="s">
+      <c r="C20" s="38"/>
+      <c r="D20" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="36" t="s">
+      <c r="E20" s="33"/>
+      <c r="F20" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="30"/>
       <c r="I20" s="26" t="s">
         <v>66</v>
       </c>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="37" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="36" t="s">
+      <c r="E21" s="33"/>
+      <c r="F21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="30"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="36" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="36"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="37" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="36" t="s">
+      <c r="E23" s="33"/>
+      <c r="F23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="37" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="36" t="s">
+      <c r="E24" s="33"/>
+      <c r="F24" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="36"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34" t="s">
+      <c r="C25" s="47"/>
+      <c r="D25" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -1860,14 +1862,14 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
@@ -1880,96 +1882,96 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="34"/>
+      <c r="D29" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35" t="s">
+      <c r="E29" s="34"/>
+      <c r="F29" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="35"/>
+      <c r="G29" s="34"/>
       <c r="I29" s="26" t="s">
         <v>67</v>
       </c>
       <c r="J29" s="26"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="37" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="36" t="s">
+      <c r="E31" s="33"/>
+      <c r="F31" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="30"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="37" t="s">
+      <c r="C32" s="31"/>
+      <c r="D32" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="36" t="s">
+      <c r="E32" s="33"/>
+      <c r="F32" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="36"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="37" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="36" t="s">
+      <c r="E33" s="33"/>
+      <c r="F33" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="36"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="34" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -1980,14 +1982,14 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
@@ -1998,141 +2000,165 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35" t="s">
+      <c r="C39" s="34"/>
+      <c r="D39" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35" t="s">
+      <c r="E39" s="34"/>
+      <c r="F39" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="35"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="37" t="s">
+      <c r="C40" s="31"/>
+      <c r="D40" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="37"/>
-      <c r="F40" s="36" t="s">
+      <c r="E40" s="33"/>
+      <c r="F40" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="36"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="37" t="s">
+      <c r="C41" s="31"/>
+      <c r="D41" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="37" t="s">
+      <c r="C42" s="31"/>
+      <c r="D42" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="37" t="s">
+      <c r="C43" s="31"/>
+      <c r="D43" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="37" t="s">
+      <c r="C44" s="32"/>
+      <c r="D44" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="36" t="s">
+      <c r="E44" s="33"/>
+      <c r="F44" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="36"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="37" t="s">
+      <c r="C45" s="31"/>
+      <c r="D45" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="37"/>
-      <c r="F45" s="36" t="s">
+      <c r="E45" s="33"/>
+      <c r="F45" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="36"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="30"/>
+      <c r="C47" s="44"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:G49"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I29:J30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="F41:G41"/>
@@ -2149,48 +2175,24 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I29:J30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:G49"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2202,7 +2204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064DA171-C1CC-439E-88B1-52F94C095D82}">
   <dimension ref="B5:L45"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2218,14 +2220,14 @@
       <c r="L5" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
       <c r="K7" s="25" t="s">
         <v>65</v>
       </c>
@@ -2244,46 +2246,46 @@
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="12"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
@@ -2349,124 +2351,124 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33" t="s">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33" t="s">
+      <c r="F20" s="47"/>
+      <c r="G20" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="38" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="36" t="s">
+      <c r="F21" s="36"/>
+      <c r="G21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="38" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="38" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="38" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="38" t="s">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="36" t="s">
+      <c r="F25" s="36"/>
+      <c r="G25" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="38" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="49" t="s">
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
       <c r="K27" s="26" t="s">
         <v>67</v>
       </c>
@@ -2484,101 +2486,101 @@
       <c r="L29" s="3"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33" t="s">
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="33" t="s">
+      <c r="H31" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="33"/>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="38" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="38"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="38" t="s">
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F36" s="38"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
+      <c r="F36" s="36"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="57">
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="50">
         <f>SUM(SUM(E33:F34),SUM(E36:F37))</f>
         <v>0</v>
       </c>
-      <c r="F38" s="57"/>
+      <c r="F38" s="50"/>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
@@ -2588,71 +2590,85 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33" t="s">
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="33"/>
+      <c r="F42" s="47"/>
       <c r="G42" s="14"/>
-      <c r="H42" s="33" t="s">
+      <c r="H42" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="I42" s="33"/>
+      <c r="I42" s="47"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36" t="s">
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F43" s="36"/>
+      <c r="F43" s="30"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="57">
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="50">
         <f>SUM(E43:F44)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="57"/>
+      <c r="F45" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="K7:L9"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K27:L28"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I44"/>
-    <mergeCell ref="H32:I37"/>
+  <mergeCells count="55">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D9:G9"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:F31"/>
@@ -2669,36 +2685,19 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="K7:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="H32:I37"/>
     <mergeCell ref="G27:I27"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2723,26 +2722,26 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -2750,12 +2749,12 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="K7" s="25" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Carta4 descargapdf y carga de datos completado
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27816"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470425EF-1C7E-4A9F-946D-C0E8C87D88EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD64A99-35E1-4AA8-BBAF-B06D29AED50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
+    <workbookView xWindow="4008" yWindow="1764" windowWidth="17280" windowHeight="9060" activeTab="3" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -588,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -634,6 +625,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -710,14 +702,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -733,14 +728,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,9 +998,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1048,7 +1038,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1154,7 +1144,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1296,7 +1286,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1306,100 +1296,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02853BE-23F3-4FDB-A85E-D2B25CE2876F}">
   <dimension ref="B8:J43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="25"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
+    <row r="15" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+    <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>3</v>
       </c>
@@ -1412,18 +1402,18 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1434,135 +1424,135 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="28" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I20" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+    <row r="23" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+    <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+    <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
+    <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+    <row r="27" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="26" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I30" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -1588,35 +1578,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8B61D0-1E0A-46E2-B36D-518440A4EA7A}">
   <dimension ref="B6:J49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:C31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1624,60 +1614,60 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="I8" s="25" t="s">
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="I8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="25"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="14"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1685,7 +1675,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
@@ -1697,7 +1687,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -1709,7 +1699,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="15" t="s">
@@ -1719,7 +1709,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1727,19 +1717,19 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1747,113 +1737,113 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="39"/>
+      <c r="G19" s="40"/>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="37" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="33" t="s">
+      <c r="C20" s="39"/>
+      <c r="D20" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="30" t="s">
+      <c r="E20" s="34"/>
+      <c r="F20" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="I20" s="26" t="s">
+      <c r="G20" s="31"/>
+      <c r="I20" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="30" t="s">
+      <c r="E21" s="34"/>
+      <c r="F21" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="31"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="33" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="30" t="s">
+      <c r="E22" s="34"/>
+      <c r="F22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="33" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="30" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="33" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="30" t="s">
+      <c r="E24" s="34"/>
+      <c r="F24" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="47" t="s">
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="35" t="s">
+      <c r="C25" s="48"/>
+      <c r="D25" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="36"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1861,19 +1851,19 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -1881,99 +1871,99 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34" t="s">
+      <c r="E29" s="35"/>
+      <c r="F29" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="I29" s="26" t="s">
+      <c r="G29" s="35"/>
+      <c r="I29" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J29" s="26"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="J29" s="27"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="33" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="30" t="s">
+      <c r="E31" s="34"/>
+      <c r="F31" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="31"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="33" t="s">
+      <c r="C32" s="32"/>
+      <c r="D32" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="30" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="33" t="s">
+      <c r="C33" s="32"/>
+      <c r="D33" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="30" t="s">
+      <c r="E33" s="34"/>
+      <c r="F33" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="30" t="s">
+      <c r="G33" s="31"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="35" t="s">
+      <c r="C35" s="31"/>
+      <c r="D35" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="36"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -1981,17 +1971,17 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="46" t="s">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -1999,121 +1989,121 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="34" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34" t="s">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34" t="s">
+      <c r="E39" s="35"/>
+      <c r="F39" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="34"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
+      <c r="G39" s="35"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="33" t="s">
+      <c r="C40" s="32"/>
+      <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="30" t="s">
+      <c r="E40" s="34"/>
+      <c r="F40" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="30"/>
-    </row>
-    <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="31" t="s">
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="33" t="s">
+      <c r="C41" s="32"/>
+      <c r="D41" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="33"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
+      <c r="E41" s="34"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="33" t="s">
+      <c r="C42" s="32"/>
+      <c r="D42" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="31" t="s">
+      <c r="E42" s="34"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="33" t="s">
+      <c r="C43" s="32"/>
+      <c r="D43" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="32" t="s">
+      <c r="E43" s="34"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="33" t="s">
+      <c r="C44" s="33"/>
+      <c r="D44" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="30" t="s">
+      <c r="E44" s="34"/>
+      <c r="F44" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="30"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="31" t="s">
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="33" t="s">
+      <c r="C45" s="32"/>
+      <c r="D45" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="30" t="s">
+      <c r="E45" s="34"/>
+      <c r="F45" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="30"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="44" t="s">
+      <c r="G45" s="31"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="44"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="45" t="s">
+      <c r="C47" s="45"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -2204,90 +2194,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064DA171-C1CC-439E-88B1-52F94C095D82}">
   <dimension ref="B5:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A30" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:F43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="K7" s="25" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="K7" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="58" t="s">
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="58" t="s">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -2295,7 +2287,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
@@ -2307,7 +2299,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +2313,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="15" t="s">
@@ -2331,320 +2323,321 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="K17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="26"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="47" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47" t="s">
+      <c r="F20" s="48"/>
+      <c r="G20" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="36" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="30" t="s">
+      <c r="F21" s="37"/>
+      <c r="G21" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="36" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="F22" s="37"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="36" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="F23" s="37"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="36" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="F24" s="37"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="36" t="s">
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="30" t="s">
+      <c r="F25" s="37"/>
+      <c r="G25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="36" t="s">
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="47" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="51" t="s">
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="K27" s="26" t="s">
+      <c r="F27" s="53"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="K27" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="26"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="27"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
         <v>98</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="47" t="s">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="47" t="s">
+      <c r="H31" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="47"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="52" t="s">
+      <c r="I31" s="48"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="54"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="36" t="s">
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="55" t="s">
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="36" t="s">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="49" t="s">
+      <c r="F36" s="37"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50">
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="51">
         <f>SUM(SUM(E33:F34),SUM(E36:F37))</f>
         <v>0</v>
       </c>
-      <c r="F38" s="50"/>
+      <c r="F38" s="51"/>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="47" t="s">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47" t="s">
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="47"/>
+      <c r="F42" s="48"/>
       <c r="G42" s="14"/>
-      <c r="H42" s="47" t="s">
+      <c r="H42" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="I42" s="47"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="30" t="s">
+      <c r="I42" s="48"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30" t="s">
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="F43" s="30"/>
+      <c r="F43" s="31"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="49" t="s">
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="50">
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="51">
         <f>SUM(E43:F44)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="50"/>
+      <c r="F45" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="B27:D27"/>
@@ -2658,46 +2651,45 @@
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="K7:L9"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:F31"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="H31:I31"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="K7:L9"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K27:L28"/>
-    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="H43:I44"/>
     <mergeCell ref="H32:I37"/>
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2709,58 +2701,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5DB1-9EBB-48B8-AAC3-58813119E4A1}">
   <dimension ref="B5:L52"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="9" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="9" width="7.5546875" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="K7" s="25" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="K7" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>72</v>
       </c>
@@ -2771,10 +2763,10 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>73</v>
       </c>
@@ -2784,10 +2776,10 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="8"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-    </row>
-    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="2:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>74</v>
       </c>
@@ -2815,7 +2807,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="20" t="s">
         <v>80</v>
       </c>
@@ -2829,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
         <v>81</v>
       </c>
@@ -2843,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="20" t="s">
         <v>82</v>
       </c>
@@ -2857,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
         <v>83</v>
       </c>
@@ -2871,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="20" t="s">
         <v>84</v>
       </c>
@@ -2887,7 +2879,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
         <v>85</v>
       </c>
@@ -2901,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
         <v>86</v>
       </c>
@@ -2919,7 +2911,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
         <v>87</v>
       </c>
@@ -2932,12 +2924,12 @@
       <c r="I18" s="20">
         <v>0</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="26"/>
-    </row>
-    <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
         <v>88</v>
       </c>
@@ -2953,7 +2945,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="20" t="s">
         <v>89</v>
       </c>
@@ -2967,25 +2959,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="21">
-        <v>21638.1</v>
-      </c>
+      <c r="C21" s="21"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="21">
-        <v>6936.58</v>
-      </c>
+      <c r="G21" s="21"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="21">
-        <v>28574.68</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
         <v>91</v>
       </c>
@@ -2999,12 +2987,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>74</v>
       </c>
@@ -3027,7 +3015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="20" t="s">
         <v>80</v>
       </c>
@@ -3040,7 +3028,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="20" t="s">
         <v>81</v>
       </c>
@@ -3051,7 +3039,7 @@
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="20" t="s">
         <v>82</v>
       </c>
@@ -3061,12 +3049,12 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="K27" s="26" t="s">
+      <c r="K27" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="26"/>
-    </row>
-    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="27"/>
+    </row>
+    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
         <v>83</v>
       </c>
@@ -3076,10 +3064,10 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+    </row>
+    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="20" t="s">
         <v>84</v>
       </c>
@@ -3092,7 +3080,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="20" t="s">
         <v>85</v>
       </c>
@@ -3103,7 +3091,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>86</v>
       </c>
@@ -3114,7 +3102,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="20" t="s">
         <v>87</v>
       </c>
@@ -3125,7 +3113,7 @@
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="20" t="s">
         <v>88</v>
       </c>
@@ -3136,7 +3124,7 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="20" t="s">
         <v>89</v>
       </c>
@@ -3147,22 +3135,18 @@
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="21">
-        <v>21557.57</v>
-      </c>
+      <c r="C35" s="21"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="21">
-        <v>4904.3100000000004</v>
-      </c>
+      <c r="G35" s="21"/>
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="20" t="s">
         <v>91</v>
       </c>
@@ -3173,12 +3157,12 @@
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="18" t="s">
         <v>74</v>
       </c>
@@ -3201,7 +3185,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="20" t="s">
         <v>80</v>
       </c>
@@ -3212,7 +3196,7 @@
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="20" t="s">
         <v>81</v>
       </c>
@@ -3223,7 +3207,7 @@
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
     </row>
-    <row r="41" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="20" t="s">
         <v>82</v>
       </c>
@@ -3234,7 +3218,7 @@
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
     </row>
-    <row r="42" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="20" t="s">
         <v>83</v>
       </c>
@@ -3245,7 +3229,7 @@
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
     </row>
-    <row r="43" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="20" t="s">
         <v>84</v>
       </c>
@@ -3256,7 +3240,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
     </row>
-    <row r="44" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="20" t="s">
         <v>85</v>
       </c>
@@ -3267,7 +3251,7 @@
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
     </row>
-    <row r="45" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="20" t="s">
         <v>86</v>
       </c>
@@ -3278,7 +3262,7 @@
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="20" t="s">
         <v>87</v>
       </c>
@@ -3289,7 +3273,7 @@
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
     </row>
-    <row r="47" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="20" t="s">
         <v>88</v>
       </c>
@@ -3300,7 +3284,7 @@
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
     </row>
-    <row r="48" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="20" t="s">
         <v>89</v>
       </c>
@@ -3311,22 +3295,18 @@
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
     </row>
-    <row r="49" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="21">
-        <v>2598.4499999999998</v>
-      </c>
+      <c r="C49" s="21"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="21">
-        <v>2341.12</v>
-      </c>
+      <c r="G49" s="21"/>
       <c r="H49" s="20"/>
     </row>
-    <row r="50" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="20" t="s">
         <v>91</v>
       </c>
@@ -3337,7 +3317,7 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="14" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
cambios solicitados por Jean a carta 4
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55500C35-0239-4554-B845-59D0240BA814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B577CDD0-9D49-4671-BF7B-F78B4CA179DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
@@ -664,6 +664,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -685,97 +686,96 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1354,84 +1354,84 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="35"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1449,11 +1449,11 @@
     </row>
     <row r="18" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1470,69 +1470,69 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="37"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="6"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
@@ -1543,14 +1543,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I30" s="37" t="s">
+      <c r="I30" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="37"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
@@ -1563,41 +1563,41 @@
       <c r="B33" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -1641,15 +1641,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
@@ -1666,55 +1666,55 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="J8" s="36" t="s">
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="J8" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="36"/>
+      <c r="K8" s="37"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="14"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1775,15 +1775,15 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -1797,117 +1797,117 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50" t="s">
+      <c r="F19" s="58"/>
+      <c r="G19" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="50"/>
+      <c r="H19" s="58"/>
       <c r="J19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="41" t="s">
+      <c r="F20" s="49"/>
+      <c r="G20" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="41"/>
-      <c r="J20" s="37" t="s">
+      <c r="H20" s="48"/>
+      <c r="J20" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="41" t="s">
+      <c r="F21" s="49"/>
+      <c r="G21" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="41"/>
+      <c r="H21" s="48"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="27"/>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="41" t="s">
+      <c r="F22" s="49"/>
+      <c r="G22" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="41"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="41" t="s">
+      <c r="F23" s="49"/>
+      <c r="G23" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="41"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="41" t="s">
+      <c r="F24" s="49"/>
+      <c r="G24" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="41"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="24"/>
       <c r="E25" s="46" t="s">
         <v>49</v>
       </c>
       <c r="F25" s="46"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
@@ -1919,15 +1919,15 @@
       <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
@@ -1941,103 +1941,103 @@
       <c r="H28" s="11"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="45"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45" t="s">
+      <c r="F29" s="47"/>
+      <c r="G29" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="45"/>
-      <c r="J29" s="37" t="s">
+      <c r="H29" s="47"/>
+      <c r="J29" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="37"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="42"/>
+      <c r="C31" s="53"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="44" t="s">
+      <c r="E31" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="44"/>
-      <c r="G31" s="41" t="s">
+      <c r="F31" s="49"/>
+      <c r="G31" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="41"/>
+      <c r="H31" s="48"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="41" t="s">
+      <c r="F32" s="49"/>
+      <c r="G32" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="41"/>
+      <c r="H32" s="48"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="42"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="27"/>
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="41" t="s">
+      <c r="F33" s="49"/>
+      <c r="G33" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="41"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="48"/>
       <c r="D35" s="26"/>
       <c r="E35" s="46" t="s">
         <v>53</v>
       </c>
       <c r="F35" s="46"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
@@ -2049,15 +2049,15 @@
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
@@ -2069,133 +2069,193 @@
       <c r="H38" s="11"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="45"/>
+      <c r="C39" s="47"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="45" t="s">
+      <c r="E39" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45" t="s">
+      <c r="F39" s="47"/>
+      <c r="G39" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="45"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="53"/>
       <c r="D40" s="27"/>
-      <c r="E40" s="44" t="s">
+      <c r="E40" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="41" t="s">
+      <c r="F40" s="49"/>
+      <c r="G40" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="41"/>
+      <c r="H40" s="48"/>
     </row>
     <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="53"/>
       <c r="D41" s="27"/>
-      <c r="E41" s="44" t="s">
+      <c r="E41" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="44"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="42"/>
+      <c r="C42" s="53"/>
       <c r="D42" s="27"/>
-      <c r="E42" s="44" t="s">
+      <c r="E42" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="42"/>
+      <c r="C43" s="53"/>
       <c r="D43" s="27"/>
-      <c r="E43" s="44" t="s">
+      <c r="E43" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="43"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="30"/>
-      <c r="E44" s="44" t="s">
+      <c r="E44" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="41" t="s">
+      <c r="F44" s="49"/>
+      <c r="G44" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="H44" s="41"/>
+      <c r="H44" s="48"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="42"/>
+      <c r="C45" s="53"/>
       <c r="D45" s="27"/>
-      <c r="E45" s="44" t="s">
+      <c r="E45" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="41" t="s">
+      <c r="F45" s="49"/>
+      <c r="G45" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="41"/>
+      <c r="H45" s="48"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="55"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J29:K30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:H49"/>
     <mergeCell ref="B17:H17"/>
@@ -2212,66 +2272,6 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="J8:K10"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J29:K30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="E45:F45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2304,15 +2304,15 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
       <c r="K4" s="33"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
@@ -2324,10 +2324,10 @@
       <c r="H5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -2337,8 +2337,8 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
@@ -2398,338 +2398,307 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="J13" s="37" t="s">
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="J13" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="47" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="41" t="s">
+      <c r="E15" s="50"/>
+      <c r="F15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="47" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="47" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="47" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="47" t="s">
+      <c r="C19" s="53"/>
+      <c r="D19" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="41" t="s">
+      <c r="E19" s="50"/>
+      <c r="F19" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="47" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="64" t="s">
+      <c r="C21" s="45"/>
+      <c r="D21" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="J21" s="37" t="s">
+      <c r="E21" s="63"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="J21" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="37"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58" t="s">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="58"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="45"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="67"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="47" t="s">
+      <c r="C25" s="53"/>
+      <c r="D25" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="47"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="47" t="s">
+      <c r="C28" s="53"/>
+      <c r="D28" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
+      <c r="E28" s="50"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="63">
+      <c r="C30" s="61"/>
+      <c r="D30" s="62">
         <f>SUM(SUM(D25:E26),SUM(D28:E29))</f>
         <v>0</v>
       </c>
-      <c r="E30" s="63"/>
+      <c r="E30" s="62"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58" t="s">
+      <c r="C32" s="45"/>
+      <c r="D32" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="58"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="58" t="s">
+      <c r="G32" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="H32" s="58"/>
+      <c r="H32" s="45"/>
     </row>
     <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="47" t="s">
+      <c r="C33" s="53"/>
+      <c r="D33" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="50"/>
       <c r="F33" s="14"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
       <c r="F34" s="14"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="63">
+      <c r="C35" s="61"/>
+      <c r="D35" s="62">
         <f>SUM(D33:E34)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="63"/>
+      <c r="E35" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="J5:K6"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G33:H34"/>
@@ -2746,12 +2715,43 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2763,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5DB1-9EBB-48B8-AAC3-58813119E4A1}">
   <dimension ref="B5:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2776,26 +2776,27 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -2803,16 +2804,16 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="K7" s="36" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="K7" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="37"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
@@ -2825,8 +2826,8 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
@@ -2838,8 +2839,8 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="8"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="2:12" ht="19.2" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
@@ -2986,10 +2987,10 @@
       <c r="I18" s="20">
         <v>0</v>
       </c>
-      <c r="K18" s="37" t="s">
+      <c r="K18" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="37"/>
+      <c r="L18" s="38"/>
     </row>
     <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
@@ -3031,7 +3032,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="71">
+      <c r="I21" s="34">
         <v>0</v>
       </c>
     </row>
@@ -3111,10 +3112,10 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="K27" s="37" t="s">
+      <c r="K27" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="37"/>
+      <c r="L27" s="38"/>
     </row>
     <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
@@ -3126,8 +3127,8 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
     </row>
     <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="20" t="s">
@@ -3389,9 +3390,9 @@
     <mergeCell ref="K7:L9"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K27:L28"/>
-    <mergeCell ref="B5:H5"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajuste de totales de las cartas
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB74340-4C4E-49C1-9F55-BE0E8FEF1200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F13EA3-5894-41A3-8724-C091543BDEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
   <si>
     <t>De nuestra consideración:</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>CGN:</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.TotalVolumenPorCliente}}</t>
+  </si>
+  <si>
+    <t>{{Osinergmin2.TotalInventarioLiquidoGasNatural}}</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -748,9 +754,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -768,9 +780,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1051,9 +1060,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1091,7 +1100,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1197,7 +1206,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1339,7 +1348,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2292,7 +2301,7 @@
   <dimension ref="B3:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,8 +2354,8 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -2406,15 +2415,15 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
       <c r="J13" s="37" t="s">
         <v>66</v>
       </c>
@@ -2526,10 +2535,10 @@
         <v>28</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="61"/>
+      <c r="E21" s="63"/>
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
@@ -2539,15 +2548,15 @@
       <c r="K21" s="37"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
@@ -2567,12 +2576,12 @@
       <c r="H23" s="44"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="14"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
@@ -2600,12 +2609,12 @@
       <c r="H26" s="44"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="65" t="s">
+      <c r="B27" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
     </row>
@@ -2622,36 +2631,35 @@
       <c r="H28" s="44"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60">
-        <f>SUM(SUM(D25:E26),SUM(D28:E29))</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="61"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="44" t="s">
@@ -2691,20 +2699,17 @@
       <c r="H34" s="47"/>
     </row>
     <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60">
-        <f>SUM(D33:E34)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="D25:E25"/>
@@ -2740,8 +2745,6 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B35:C35"/>
@@ -2756,10 +2759,14 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2799,11 +2806,11 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>

</xml_diff>

<commit_message>
actualización de página 5 y 6
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F13EA3-5894-41A3-8724-C091543BDEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E399AF2-86F6-4160-92E3-B683CB05D918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja2 (2)" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Osinergmin2_Cgn">Hoja4!$B$28:$E$29</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="157">
   <si>
     <t>De nuestra consideración:</t>
   </si>
@@ -415,12 +416,140 @@
   <si>
     <t>{{Osinergmin2.TotalInventarioLiquidoGasNatural}}</t>
   </si>
+  <si>
+    <t>PLANTA DE GAS TALARA</t>
+  </si>
+  <si>
+    <t>REPORTE ANÁLISIS CROMATOGRÁFICO</t>
+  </si>
+  <si>
+    <t>Procedencia Gas Asociado:</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>LOTE Z - 2B/Z - 69 - SAVIA/PETROPERU</t>
+  </si>
+  <si>
+    <t>LOTE VI - PETROPERU</t>
+  </si>
+  <si>
+    <t>LOTE X - CNPC PERÚ S.A.</t>
+  </si>
+  <si>
+    <t>LOTE IV - UNNA ENERGIA</t>
+  </si>
+  <si>
+    <t>LOTE I - PETROPERU</t>
+  </si>
+  <si>
+    <t>NOVIEMBRE DEL 2023</t>
+  </si>
+  <si>
+    <t>Preparado</t>
+  </si>
+  <si>
+    <t>Propiedades:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Método ASTM
+D-2163</t>
+  </si>
+  <si>
+    <t>Composición % Molar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOTE Z - 2B / Z - 69 </t>
+  </si>
+  <si>
+    <t>LOTE X</t>
+  </si>
+  <si>
+    <t>Lote VII - VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOTE I</t>
+  </si>
+  <si>
+    <t>UNNA LOTE IV</t>
+  </si>
+  <si>
+    <t>Metano</t>
+  </si>
+  <si>
+    <t>Etano</t>
+  </si>
+  <si>
+    <t>Propano</t>
+  </si>
+  <si>
+    <t>Iso-Butano</t>
+  </si>
+  <si>
+    <t>Normal-Butano</t>
+  </si>
+  <si>
+    <t>Neo-Pentano</t>
+  </si>
+  <si>
+    <t>Iso-Pentano</t>
+  </si>
+  <si>
+    <t>Normal-Pentano</t>
+  </si>
+  <si>
+    <t>Hexano +</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>BTU (Bruto)</t>
+  </si>
+  <si>
+    <t>BTU (Neto)</t>
+  </si>
+  <si>
+    <t>Grav. Espec.</t>
+  </si>
+  <si>
+    <t>Gal. LGN/mpc</t>
+  </si>
+  <si>
+    <t>Peso Molec.</t>
+  </si>
+  <si>
+    <t>PREPARADO POR :</t>
+  </si>
+  <si>
+    <t>APROBADO POR :</t>
+  </si>
+  <si>
+    <t>REPORTES</t>
+  </si>
+  <si>
+    <t>Jean Asanza Rosales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Original:
+c.c. Arch. Laboratorio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,16 +640,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF3F4254"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -598,11 +741,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -679,6 +914,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -754,44 +1033,100 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,10 +1394,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>70418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>732839</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>46606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA71E8C-369C-4954-83A5-31C23A43266A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="327080" y="70418"/>
+          <a:ext cx="1472559" cy="547688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1100,7 +1484,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1206,7 +1590,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1348,7 +1732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1371,84 +1755,84 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="35"/>
+      <c r="G9" s="51"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="52"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1466,11 +1850,11 @@
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1487,69 +1871,69 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="55"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="37"/>
+      <c r="J21" s="53"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="6"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -1560,14 +1944,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="37" t="s">
+      <c r="I30" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="37"/>
+      <c r="J30" s="53"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
@@ -1580,41 +1964,41 @@
       <c r="B33" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -1641,7 +2025,7 @@
   <dimension ref="B6:K49"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H6"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,15 +2042,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
@@ -1683,55 +2067,55 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="J8" s="36" t="s">
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="J8" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="36"/>
+      <c r="K8" s="52"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="14"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1792,15 +2176,15 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -1814,117 +2198,117 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="57"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57" t="s">
+      <c r="F19" s="73"/>
+      <c r="G19" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="57"/>
+      <c r="H19" s="73"/>
       <c r="J19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="47" t="s">
+      <c r="F20" s="64"/>
+      <c r="G20" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="47"/>
-      <c r="J20" s="37" t="s">
+      <c r="H20" s="63"/>
+      <c r="J20" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="52"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="47" t="s">
+      <c r="F21" s="64"/>
+      <c r="G21" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="47"/>
+      <c r="H21" s="63"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="52"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="27"/>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="47" t="s">
+      <c r="F22" s="64"/>
+      <c r="G22" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="47"/>
+      <c r="H22" s="63"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="47" t="s">
+      <c r="F23" s="64"/>
+      <c r="G23" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="47"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="68"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="47" t="s">
+      <c r="F24" s="64"/>
+      <c r="G24" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="47"/>
+      <c r="H24" s="63"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="44"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="24"/>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -1936,15 +2320,15 @@
       <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
@@ -1958,103 +2342,103 @@
       <c r="H28" s="11"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="46"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="46" t="s">
+      <c r="E29" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46" t="s">
+      <c r="F29" s="62"/>
+      <c r="G29" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="J29" s="37" t="s">
+      <c r="H29" s="62"/>
+      <c r="J29" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="37"/>
+      <c r="K29" s="53"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="52"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="47" t="s">
+      <c r="F31" s="64"/>
+      <c r="G31" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="47"/>
+      <c r="H31" s="63"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="52"/>
+      <c r="C32" s="68"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="48"/>
-      <c r="G32" s="47" t="s">
+      <c r="F32" s="64"/>
+      <c r="G32" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="47"/>
+      <c r="H32" s="63"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="52"/>
+      <c r="C33" s="68"/>
       <c r="D33" s="27"/>
-      <c r="E33" s="48" t="s">
+      <c r="E33" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="48"/>
-      <c r="G33" s="47" t="s">
+      <c r="F33" s="64"/>
+      <c r="G33" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="47"/>
+      <c r="H33" s="63"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="47"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -2066,15 +2450,15 @@
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
@@ -2086,130 +2470,130 @@
       <c r="H38" s="11"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="46"/>
+      <c r="C39" s="62"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46" t="s">
+      <c r="F39" s="62"/>
+      <c r="G39" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="46"/>
+      <c r="H39" s="62"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="52"/>
+      <c r="C40" s="68"/>
       <c r="D40" s="27"/>
-      <c r="E40" s="48" t="s">
+      <c r="E40" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="48"/>
-      <c r="G40" s="47" t="s">
+      <c r="F40" s="64"/>
+      <c r="G40" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="47"/>
+      <c r="H40" s="63"/>
     </row>
     <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="52"/>
+      <c r="C41" s="68"/>
       <c r="D41" s="27"/>
-      <c r="E41" s="48" t="s">
+      <c r="E41" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="48"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="52"/>
+      <c r="C42" s="68"/>
       <c r="D42" s="27"/>
-      <c r="E42" s="48" t="s">
+      <c r="E42" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="48"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="52"/>
+      <c r="C43" s="68"/>
       <c r="D43" s="27"/>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="58"/>
+      <c r="C44" s="74"/>
       <c r="D44" s="30"/>
-      <c r="E44" s="48" t="s">
+      <c r="E44" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="48"/>
-      <c r="G44" s="47" t="s">
+      <c r="F44" s="64"/>
+      <c r="G44" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H44" s="47"/>
+      <c r="H44" s="63"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="52"/>
+      <c r="C45" s="68"/>
       <c r="D45" s="27"/>
-      <c r="E45" s="48" t="s">
+      <c r="E45" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="48"/>
-      <c r="G45" s="47" t="s">
+      <c r="F45" s="64"/>
+      <c r="G45" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="47"/>
+      <c r="H45" s="63"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="41"/>
+      <c r="C47" s="57"/>
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -2300,7 +2684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064DA171-C1CC-439E-88B1-52F94C095D82}">
   <dimension ref="B3:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2321,15 +2705,15 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
       <c r="K4" s="33"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2341,10 +2725,10 @@
       <c r="H5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="53"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -2354,8 +2738,8 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -2415,313 +2799,321 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="J13" s="37" t="s">
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="J13" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="53"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44" t="s">
+      <c r="C14" s="60"/>
+      <c r="D14" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="49" t="s">
+      <c r="C15" s="68"/>
+      <c r="D15" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="47" t="s">
+      <c r="E15" s="65"/>
+      <c r="F15" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="16" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="49" t="s">
+      <c r="C16" s="68"/>
+      <c r="D16" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="49" t="s">
+      <c r="C17" s="68"/>
+      <c r="D17" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="49" t="s">
+      <c r="C18" s="68"/>
+      <c r="D18" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="49" t="s">
+      <c r="C19" s="68"/>
+      <c r="D19" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="47" t="s">
+      <c r="E19" s="65"/>
+      <c r="F19" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="49" t="s">
+      <c r="C20" s="68"/>
+      <c r="D20" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="63" t="s">
+      <c r="C21" s="60"/>
+      <c r="D21" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="J21" s="37" t="s">
+      <c r="E21" s="77"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="J21" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="37"/>
+      <c r="K21" s="53"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44" t="s">
+      <c r="C23" s="60"/>
+      <c r="D23" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="44" t="s">
+      <c r="G23" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="44"/>
+      <c r="H23" s="60"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="66"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="80"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="49" t="s">
+      <c r="C25" s="68"/>
+      <c r="D25" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="49"/>
+      <c r="E25" s="65"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="49" t="s">
+      <c r="C28" s="68"/>
+      <c r="D28" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
+      <c r="E28" s="65"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61" t="s">
+      <c r="C30" s="75"/>
+      <c r="D30" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="61"/>
+      <c r="E30" s="85"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44" t="s">
+      <c r="C32" s="60"/>
+      <c r="D32" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="44"/>
+      <c r="E32" s="60"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="44" t="s">
+      <c r="G32" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="H32" s="44"/>
+      <c r="H32" s="60"/>
     </row>
     <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="52"/>
-      <c r="D33" s="49" t="s">
+      <c r="C33" s="68"/>
+      <c r="D33" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="49"/>
+      <c r="E33" s="65"/>
       <c r="F33" s="14"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
     </row>
     <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
       <c r="F34" s="14"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
     </row>
     <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="62" t="s">
+      <c r="C35" s="75"/>
+      <c r="D35" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="62"/>
+      <c r="E35" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="J5:K6"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G33:H34"/>
     <mergeCell ref="G24:H29"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B31:H31"/>
-    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="J13:K13"/>
@@ -2734,16 +3126,15 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D20:E20"/>
@@ -2760,13 +3151,6 @@
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2791,26 +3175,26 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -2818,16 +3202,16 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="K7" s="36" t="s">
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="K7" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="52"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
@@ -2840,8 +3224,8 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
@@ -2853,8 +3237,8 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="8"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
@@ -3001,10 +3385,10 @@
       <c r="I18" s="20">
         <v>0</v>
       </c>
-      <c r="K18" s="37" t="s">
+      <c r="K18" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="37"/>
+      <c r="L18" s="53"/>
     </row>
     <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
@@ -3130,10 +3514,10 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="K27" s="37" t="s">
+      <c r="K27" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="37"/>
+      <c r="L27" s="53"/>
     </row>
     <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
@@ -3145,8 +3529,8 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
     </row>
     <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
@@ -3424,4 +3808,704 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A076B2-8FC6-42F9-BD63-7589A58CEBFA}">
+  <dimension ref="B5:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="93" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="107" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+    </row>
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="J8" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="52"/>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="91" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="91" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="88" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="105" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="102" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="103" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="104" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="97" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="40">
+        <v>87.411500000000004</v>
+      </c>
+      <c r="E17" s="40">
+        <v>91.2881</v>
+      </c>
+      <c r="F17" s="40">
+        <v>84.917299999999997</v>
+      </c>
+      <c r="G17" s="40">
+        <v>84.561400000000006</v>
+      </c>
+      <c r="H17" s="44">
+        <v>90.105099999999993</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43">
+        <v>6.9951999999999996</v>
+      </c>
+      <c r="E18" s="43">
+        <v>3.5409000000000002</v>
+      </c>
+      <c r="F18" s="43">
+        <v>6.5328999999999997</v>
+      </c>
+      <c r="G18" s="43">
+        <v>6.6307</v>
+      </c>
+      <c r="H18" s="45">
+        <v>4.1820000000000004</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="53"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
+        <v>1.5104</v>
+      </c>
+      <c r="E19" s="43">
+        <v>1.5378000000000001</v>
+      </c>
+      <c r="F19" s="43">
+        <v>3.5259999999999998</v>
+      </c>
+      <c r="G19" s="43">
+        <v>3.6059999999999999</v>
+      </c>
+      <c r="H19" s="45">
+        <v>2.1492</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43">
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="E20" s="43">
+        <v>0.62709999999999999</v>
+      </c>
+      <c r="F20" s="43">
+        <v>1.0871</v>
+      </c>
+      <c r="G20" s="43">
+        <v>1.0502</v>
+      </c>
+      <c r="H20" s="45">
+        <v>0.81540000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43">
+        <v>0.74639999999999995</v>
+      </c>
+      <c r="E21" s="43">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="F21" s="43">
+        <v>1.5216000000000001</v>
+      </c>
+      <c r="G21" s="43">
+        <v>1.4770000000000001</v>
+      </c>
+      <c r="H21" s="45">
+        <v>1.0411999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43">
+        <v>0</v>
+      </c>
+      <c r="E22" s="43">
+        <v>0</v>
+      </c>
+      <c r="F22" s="43">
+        <v>0</v>
+      </c>
+      <c r="G22" s="43">
+        <v>0</v>
+      </c>
+      <c r="H22" s="45">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43">
+        <v>0.36820000000000003</v>
+      </c>
+      <c r="E23" s="43">
+        <v>0.44479999999999997</v>
+      </c>
+      <c r="F23" s="43">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="G23" s="43">
+        <v>0.62390000000000001</v>
+      </c>
+      <c r="H23" s="45">
+        <v>0.35920000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43">
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="E24" s="43">
+        <v>0.2591</v>
+      </c>
+      <c r="F24" s="43">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="G24" s="43">
+        <v>0.37880000000000003</v>
+      </c>
+      <c r="H24" s="45">
+        <v>0.47610000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43">
+        <v>0.48449999999999999</v>
+      </c>
+      <c r="E25" s="43">
+        <v>0.66</v>
+      </c>
+      <c r="F25" s="43">
+        <v>0.7974</v>
+      </c>
+      <c r="G25" s="43">
+        <v>0.58230000000000004</v>
+      </c>
+      <c r="H25" s="45">
+        <v>0.3619</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43">
+        <v>1.5663</v>
+      </c>
+      <c r="E26" s="43">
+        <v>0.74139999999999995</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0.23930000000000001</v>
+      </c>
+      <c r="G26" s="43">
+        <v>0.67269999999999996</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0.25119999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43">
+        <v>0</v>
+      </c>
+      <c r="E27" s="43">
+        <v>0</v>
+      </c>
+      <c r="F27" s="43">
+        <v>0</v>
+      </c>
+      <c r="G27" s="43">
+        <v>0</v>
+      </c>
+      <c r="H27" s="45">
+        <v>0</v>
+      </c>
+      <c r="J27" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="53"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48">
+        <v>0.18090000000000001</v>
+      </c>
+      <c r="E28" s="48">
+        <v>0.13</v>
+      </c>
+      <c r="F28" s="48">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G28" s="48">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="H28" s="49">
+        <v>0.24709999999999999</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="43">
+        <v>100</v>
+      </c>
+      <c r="E29" s="43">
+        <v>100</v>
+      </c>
+      <c r="F29" s="43">
+        <v>100</v>
+      </c>
+      <c r="G29" s="43">
+        <v>100</v>
+      </c>
+      <c r="H29" s="43">
+        <v>100</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="40">
+        <v>1138.31</v>
+      </c>
+      <c r="E30" s="40">
+        <v>1128.83</v>
+      </c>
+      <c r="F30" s="40">
+        <v>1237.03</v>
+      </c>
+      <c r="G30" s="40">
+        <v>1219.71</v>
+      </c>
+      <c r="H30" s="40">
+        <v>1154.8399999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="43">
+        <v>1024.3399999999999</v>
+      </c>
+      <c r="E31" s="43">
+        <v>1020.25</v>
+      </c>
+      <c r="F31" s="43">
+        <v>1113.48</v>
+      </c>
+      <c r="G31" s="43">
+        <v>1098.57</v>
+      </c>
+      <c r="H31" s="43">
+        <v>1039.99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="D32" s="43">
+        <v>96.666700000000006</v>
+      </c>
+      <c r="E32" s="43">
+        <v>100</v>
+      </c>
+      <c r="F32" s="43">
+        <v>96.666700000000006</v>
+      </c>
+      <c r="G32" s="43">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="H32" s="43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43">
+        <v>1.2522</v>
+      </c>
+      <c r="E33" s="43">
+        <v>1.415</v>
+      </c>
+      <c r="F33" s="43">
+        <v>2.5529999999999999</v>
+      </c>
+      <c r="G33" s="43">
+        <v>2.4226000000000001</v>
+      </c>
+      <c r="H33" s="43">
+        <v>1.6528</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="47"/>
+      <c r="D34" s="48">
+        <v>19.1113</v>
+      </c>
+      <c r="E34" s="48">
+        <v>18.6401</v>
+      </c>
+      <c r="F34" s="48">
+        <v>20.318000000000001</v>
+      </c>
+      <c r="G34" s="48">
+        <v>20.257200000000001</v>
+      </c>
+      <c r="H34" s="48">
+        <v>18.842600000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="57"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="92"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="92"/>
+      <c r="H37" s="92"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="92"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="92"/>
+      <c r="E38" s="92"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="92"/>
+    </row>
+    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="62"/>
+      <c r="F40" s="90" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="94"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="G41" s="96"/>
+      <c r="H41" s="96"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="94"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="96"/>
+      <c r="H43" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="J8:K10"/>
+    <mergeCell ref="B41:C43"/>
+    <mergeCell ref="D41:E43"/>
+    <mergeCell ref="F41:H43"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="J27:K28"/>
+    <mergeCell ref="F10:H11"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:H38"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F12:H14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:H40"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste de reporte página 4
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/cartas/solicitud.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN_02\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\cartas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E399AF2-86F6-4160-92E3-B683CB05D918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66C9546-AAFB-4B7A-8205-44C86EAFBA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C8FC5450-17C5-4C27-BE32-326C1CD393B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja2 (2)" sheetId="5" r:id="rId5"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
+    <sheet name="Página2" sheetId="2" r:id="rId2"/>
+    <sheet name="Página3" sheetId="4" r:id="rId3"/>
+    <sheet name="Página4" sheetId="6" r:id="rId4"/>
+    <sheet name="Página5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Osinergmin2_Cgn">Hoja4!$B$28:$E$29</definedName>
-    <definedName name="Osinergmin2_Glp">Hoja4!$B$25:$E$26</definedName>
-    <definedName name="Osinergmin2_InventarioLiquidoGasNatural">Hoja4!$B$33:$E$34</definedName>
+    <definedName name="Osinergmin2_Cgn">Página3!$B$28:$E$29</definedName>
+    <definedName name="Osinergmin2_Glp">Página3!$B$25:$E$26</definedName>
+    <definedName name="Osinergmin2_InventarioLiquidoGasNatural">Página3!$B$33:$E$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -958,6 +958,12 @@
     <xf numFmtId="164" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1072,61 +1078,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1347,25 +1345,20 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>448255</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1471093" cy="547688"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C7D3CA-66E6-4EFE-8F0D-05C8E54D2BC3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFAA99E7-8918-4F4F-B84B-4537995985DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1382,7 +1375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="323850" y="200025"/>
-          <a:ext cx="1472559" cy="547688"/>
+          <a:ext cx="1471093" cy="547688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1390,7 +1383,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1755,84 +1748,84 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="51"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="52" t="s">
+      <c r="I9" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="52"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1850,11 +1843,11 @@
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1871,69 +1864,69 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="53"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
       <c r="H27" s="6"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -1944,14 +1937,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="53" t="s">
+      <c r="I30" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="53"/>
+      <c r="J30" s="57"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
@@ -1964,41 +1957,41 @@
       <c r="B33" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="4"/>
     </row>
   </sheetData>
@@ -2024,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8B61D0-1E0A-46E2-B36D-518440A4EA7A}">
   <dimension ref="B6:K49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,15 +2035,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
@@ -2067,55 +2060,55 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="J8" s="52" t="s">
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="J8" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="52"/>
+      <c r="K8" s="56"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="14"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -2176,15 +2169,15 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -2198,117 +2191,117 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="73"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="73" t="s">
+      <c r="E19" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73" t="s">
+      <c r="F19" s="77"/>
+      <c r="G19" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="77"/>
       <c r="J19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="72"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="64" t="s">
+      <c r="E20" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="64"/>
-      <c r="G20" s="63" t="s">
+      <c r="F20" s="68"/>
+      <c r="G20" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="63"/>
-      <c r="J20" s="53" t="s">
+      <c r="H20" s="67"/>
+      <c r="J20" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="53"/>
+      <c r="K20" s="57"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="68"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="64" t="s">
+      <c r="E21" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="64"/>
-      <c r="G21" s="63" t="s">
+      <c r="F21" s="68"/>
+      <c r="G21" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="63"/>
+      <c r="H21" s="67"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="68"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="27"/>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="63" t="s">
+      <c r="F22" s="68"/>
+      <c r="G22" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="63"/>
+      <c r="H22" s="67"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="68"/>
+      <c r="C23" s="72"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="64" t="s">
+      <c r="E23" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="64"/>
-      <c r="G23" s="63" t="s">
+      <c r="F23" s="68"/>
+      <c r="G23" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="63"/>
+      <c r="H23" s="67"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="68"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="64" t="s">
+      <c r="E24" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="64"/>
-      <c r="G24" s="63" t="s">
+      <c r="F24" s="68"/>
+      <c r="G24" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="63"/>
+      <c r="H24" s="67"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="60"/>
+      <c r="C25" s="64"/>
       <c r="D25" s="24"/>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -2320,15 +2313,15 @@
       <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
@@ -2342,103 +2335,103 @@
       <c r="H28" s="11"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="62" t="s">
+      <c r="E29" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62" t="s">
+      <c r="F29" s="66"/>
+      <c r="G29" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="62"/>
-      <c r="J29" s="53" t="s">
+      <c r="H29" s="66"/>
+      <c r="J29" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="53"/>
+      <c r="K29" s="57"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="68"/>
+      <c r="C31" s="72"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="64" t="s">
+      <c r="E31" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="64"/>
-      <c r="G31" s="63" t="s">
+      <c r="F31" s="68"/>
+      <c r="G31" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="63"/>
+      <c r="H31" s="67"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="68"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="64" t="s">
+      <c r="E32" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="64"/>
-      <c r="G32" s="63" t="s">
+      <c r="F32" s="68"/>
+      <c r="G32" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="63"/>
+      <c r="H32" s="67"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="27"/>
-      <c r="E33" s="64" t="s">
+      <c r="E33" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="64"/>
-      <c r="G33" s="63" t="s">
+      <c r="F33" s="68"/>
+      <c r="G33" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="63"/>
+      <c r="H33" s="67"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="63"/>
+      <c r="C35" s="67"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="61"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="67"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -2450,15 +2443,15 @@
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
@@ -2470,130 +2463,130 @@
       <c r="H38" s="11"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="62"/>
+      <c r="C39" s="66"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="62"/>
-      <c r="G39" s="62" t="s">
+      <c r="F39" s="66"/>
+      <c r="G39" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="62"/>
+      <c r="H39" s="66"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="68" t="s">
+      <c r="B40" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="68"/>
+      <c r="C40" s="72"/>
       <c r="D40" s="27"/>
-      <c r="E40" s="64" t="s">
+      <c r="E40" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="64"/>
-      <c r="G40" s="63" t="s">
+      <c r="F40" s="68"/>
+      <c r="G40" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="63"/>
+      <c r="H40" s="67"/>
     </row>
     <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="68" t="s">
+      <c r="B41" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="68"/>
+      <c r="C41" s="72"/>
       <c r="D41" s="27"/>
-      <c r="E41" s="64" t="s">
+      <c r="E41" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="64"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="68"/>
+      <c r="C42" s="72"/>
       <c r="D42" s="27"/>
-      <c r="E42" s="64" t="s">
+      <c r="E42" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="64"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="68"/>
+      <c r="C43" s="72"/>
       <c r="D43" s="27"/>
-      <c r="E43" s="64" t="s">
+      <c r="E43" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="F43" s="64"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="74" t="s">
+      <c r="B44" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="74"/>
+      <c r="C44" s="78"/>
       <c r="D44" s="30"/>
-      <c r="E44" s="64" t="s">
+      <c r="E44" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="64"/>
-      <c r="G44" s="63" t="s">
+      <c r="F44" s="68"/>
+      <c r="G44" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="H44" s="63"/>
+      <c r="H44" s="67"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="68"/>
+      <c r="C45" s="72"/>
       <c r="D45" s="27"/>
-      <c r="E45" s="64" t="s">
+      <c r="E45" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="64"/>
-      <c r="G45" s="63" t="s">
+      <c r="F45" s="68"/>
+      <c r="G45" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="63"/>
+      <c r="H45" s="67"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="57"/>
+      <c r="C47" s="61"/>
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -2685,7 +2678,7 @@
   <dimension ref="B3:K35"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D20" sqref="D20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,15 +2698,15 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
       <c r="K4" s="33"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2725,10 +2718,10 @@
       <c r="H5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="53"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -2738,8 +2731,8 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -2799,302 +2792,301 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="J13" s="53" t="s">
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="J13" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="53"/>
+      <c r="K13" s="57"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60" t="s">
+      <c r="E14" s="64"/>
+      <c r="F14" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="65" t="s">
+      <c r="C15" s="72"/>
+      <c r="D15" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="63" t="s">
+      <c r="E15" s="69"/>
+      <c r="F15" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
     </row>
     <row r="16" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="65" t="s">
+      <c r="C16" s="72"/>
+      <c r="D16" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="65" t="s">
+      <c r="C17" s="72"/>
+      <c r="D17" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="65" t="s">
+      <c r="C18" s="72"/>
+      <c r="D18" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="65" t="s">
+      <c r="C19" s="72"/>
+      <c r="D19" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="63" t="s">
+      <c r="E19" s="69"/>
+      <c r="F19" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="65" t="s">
+      <c r="C20" s="72"/>
+      <c r="D20" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="77" t="s">
+      <c r="C21" s="64"/>
+      <c r="D21" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="J21" s="53" t="s">
+      <c r="E21" s="81"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="J21" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="53"/>
+      <c r="K21" s="57"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60" t="s">
+      <c r="C23" s="64"/>
+      <c r="D23" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="60"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="60"/>
+      <c r="H23" s="64"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="80"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="84"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="65" t="s">
+      <c r="C25" s="72"/>
+      <c r="D25" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="65" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
+      <c r="E28" s="69"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="85" t="s">
+      <c r="C30" s="79"/>
+      <c r="D30" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="85"/>
+      <c r="E30" s="89"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="86" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60" t="s">
+      <c r="C32" s="64"/>
+      <c r="D32" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="60"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="60" t="s">
+      <c r="G32" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="H32" s="60"/>
+      <c r="H32" s="64"/>
     </row>
     <row r="33" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="65" t="s">
+      <c r="C33" s="72"/>
+      <c r="D33" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="65"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="14"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
     </row>
     <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="14"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
     </row>
     <row r="35" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="75"/>
-      <c r="D35" s="76" t="s">
+      <c r="C35" s="79"/>
+      <c r="D35" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="76"/>
+      <c r="E35" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="J5:K6"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="D19:E19"/>
@@ -3114,6 +3106,7 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="J13:K13"/>
@@ -3159,11 +3152,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5DB1-9EBB-48B8-AAC3-58813119E4A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1594384C-AFF0-46C1-A7A9-108400135801}">
   <dimension ref="B5:L52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,26 +3168,27 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -3202,16 +3196,16 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="K7" s="52" t="s">
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="K7" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="52"/>
+      <c r="L7" s="56"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
@@ -3224,8 +3218,8 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
@@ -3237,8 +3231,8 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="8"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
@@ -3385,10 +3379,10 @@
       <c r="I18" s="20">
         <v>0</v>
       </c>
-      <c r="K18" s="53" t="s">
+      <c r="K18" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="L18" s="53"/>
+      <c r="L18" s="57"/>
     </row>
     <row r="19" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
@@ -3424,18 +3418,14 @@
       <c r="B21" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="21">
-        <v>21638.1</v>
-      </c>
+      <c r="C21" s="21"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="21">
-        <v>6936.58</v>
-      </c>
+      <c r="G21" s="21"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="21">
-        <v>28574.68</v>
+      <c r="I21" s="53">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3514,10 +3504,10 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="K27" s="53" t="s">
+      <c r="K27" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="53"/>
+      <c r="L27" s="57"/>
     </row>
     <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
@@ -3529,8 +3519,8 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
     </row>
     <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
@@ -3604,15 +3594,11 @@
       <c r="B35" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="21">
-        <v>21557.57</v>
-      </c>
+      <c r="C35" s="21"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="21">
-        <v>4904.3100000000004</v>
-      </c>
+      <c r="G35" s="21"/>
       <c r="H35" s="20"/>
     </row>
     <row r="36" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3768,15 +3754,11 @@
       <c r="B49" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="21">
-        <v>2598.4499999999998</v>
-      </c>
+      <c r="C49" s="21"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="21">
-        <v>2341.12</v>
-      </c>
+      <c r="G49" s="21"/>
       <c r="H49" s="20"/>
     </row>
     <row r="50" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3797,10 +3779,10 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="K7:L9"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K27:L28"/>
-    <mergeCell ref="B5:H5"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="D6:F6"/>
   </mergeCells>
@@ -3814,7 +3796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A076B2-8FC6-42F9-BD63-7589A58CEBFA}">
   <dimension ref="B5:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
@@ -3832,158 +3814,158 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="100"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="J8" s="52" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="J8" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="52"/>
+      <c r="K8" s="56"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="99" t="s">
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="93" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="88" t="s">
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="91"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95"/>
       <c r="I11" s="14"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="88" t="s">
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="97" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="100" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="100"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
       <c r="D16" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="97" t="s">
+      <c r="E16" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="97" t="s">
+      <c r="F16" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="97" t="s">
+      <c r="G16" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="97" t="s">
+      <c r="H16" s="50" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4032,10 +4014,10 @@
       <c r="H18" s="45">
         <v>4.1820000000000004</v>
       </c>
-      <c r="J18" s="53" t="s">
+      <c r="J18" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="53"/>
+      <c r="K18" s="57"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="41" t="s">
@@ -4229,10 +4211,10 @@
       <c r="H27" s="45">
         <v>0</v>
       </c>
-      <c r="J27" s="53" t="s">
+      <c r="J27" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="53"/>
+      <c r="K27" s="57"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="46" t="s">
@@ -4254,8 +4236,8 @@
       <c r="H28" s="49">
         <v>0.24709999999999999</v>
       </c>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
@@ -4395,31 +4377,31 @@
       <c r="H35" s="36"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="23"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="92" t="s">
+      <c r="B37" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="105"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="92"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="92"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="105"/>
     </row>
     <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
@@ -4431,50 +4413,50 @@
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="62" t="s">
+      <c r="B40" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62" t="s">
+      <c r="C40" s="66"/>
+      <c r="D40" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="62"/>
-      <c r="F40" s="90" t="s">
+      <c r="E40" s="66"/>
+      <c r="F40" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="G40" s="90"/>
-      <c r="H40" s="90"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="94" t="s">
+      <c r="B41" s="102" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="94"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="95" t="s">
+      <c r="C41" s="102"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="G41" s="96"/>
-      <c r="H41" s="96"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="94"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="102"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="104"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="96"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -4494,6 +4476,8 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:H40"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
@@ -4501,8 +4485,6 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:H40"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>